<commit_message>
hyo_bodyupT and hyo_body16upT results
</commit_message>
<xml_diff>
--- a/RunParameters.xlsx
+++ b/RunParameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
   </bookViews>
   <sheets>
     <sheet name="Run parameters" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3125" uniqueCount="1357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3130" uniqueCount="1357">
   <si>
     <t>data set</t>
   </si>
@@ -31406,7 +31406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
@@ -33306,8 +33306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33477,16 +33477,36 @@
       <c r="B5" s="26" t="s">
         <v>999</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="74"/>
+      <c r="C5" s="27">
+        <v>-2708.69</v>
+      </c>
+      <c r="D5" s="27">
+        <v>-2708.9</v>
+      </c>
+      <c r="E5" s="27">
+        <v>1.24</v>
+      </c>
+      <c r="F5" s="27">
+        <v>-1</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="H5" s="77" t="s">
+        <v>965</v>
+      </c>
+      <c r="I5" s="78" t="s">
+        <v>336</v>
+      </c>
+      <c r="J5" s="29">
+        <v>0.214</v>
+      </c>
+      <c r="K5" s="29">
+        <v>0.79</v>
+      </c>
+      <c r="L5" s="74">
+        <v>7.4999999999999997E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:13" s="26" customFormat="1">
       <c r="B6" s="26" t="s">
@@ -33527,16 +33547,36 @@
       <c r="B7" s="26" t="s">
         <v>1001</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="74"/>
+      <c r="C7" s="27">
+        <v>-2698.25</v>
+      </c>
+      <c r="D7" s="27">
+        <v>-2704.9524999999999</v>
+      </c>
+      <c r="E7" s="27">
+        <v>12</v>
+      </c>
+      <c r="F7" s="27">
+        <v>-1</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>351</v>
+      </c>
+      <c r="H7" s="77" t="s">
+        <v>963</v>
+      </c>
+      <c r="I7" s="78">
+        <v>11.269</v>
+      </c>
+      <c r="J7" s="29">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="K7" s="29">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="L7" s="74">
+        <v>1.4999999999999999E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:13" s="26" customFormat="1">
       <c r="B8" s="26" t="s">

</xml_diff>

<commit_message>
hyo_bodydownT results and PartitionFinder files
</commit_message>
<xml_diff>
--- a/RunParameters.xlsx
+++ b/RunParameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Run parameters" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3130" uniqueCount="1357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3133" uniqueCount="1358">
   <si>
     <t>data set</t>
   </si>
@@ -30727,6 +30727,9 @@
       </rPr>
       <t>). SB I reverses the trajectory to counter-clockwise, but SB II immediately restores it to clockwise. Both are either absent or present simultaneously in all taxa considered in this study and are thus treated as a single character.</t>
     </r>
+  </si>
+  <si>
+    <t>0.4</t>
   </si>
 </sst>
 </file>
@@ -31406,9 +31409,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1:Q1048576"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33304,10 +33307,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33322,7 +33328,7 @@
     <col min="9" max="9" width="6.85546875" style="61" customWidth="1"/>
     <col min="10" max="11" width="8.5703125" style="7" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" style="73" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="2" hidden="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -33582,16 +33588,36 @@
       <c r="B8" s="26" t="s">
         <v>1002</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="74"/>
+      <c r="C8" s="27">
+        <v>-2708.63</v>
+      </c>
+      <c r="D8" s="27">
+        <v>-2709.0075000000002</v>
+      </c>
+      <c r="E8" s="27">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="F8" s="27">
+        <v>-1</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="H8" s="77" t="s">
+        <v>1357</v>
+      </c>
+      <c r="I8" s="78" t="s">
+        <v>336</v>
+      </c>
+      <c r="J8" s="29">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="K8" s="29">
+        <v>0.79</v>
+      </c>
+      <c r="L8" s="74">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="9" spans="1:13" s="16" customFormat="1">
       <c r="B9" s="16" t="s">
@@ -34858,7 +34884,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="72" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ss runs from prior
</commit_message>
<xml_diff>
--- a/RunParameters.xlsx
+++ b/RunParameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Run parameters" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3135" uniqueCount="1360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3141" uniqueCount="1365">
   <si>
     <t>data set</t>
   </si>
@@ -30736,6 +30736,21 @@
   </si>
   <si>
     <t>The two arms of the switchback may be separated, or so close that they nearly touch.</t>
+  </si>
+  <si>
+    <t>hyo_bodyFP_ss.nex</t>
+  </si>
+  <si>
+    <t>hyo_neotransFP_ss.nex</t>
+  </si>
+  <si>
+    <t>hyo_devFP_ss.nex</t>
+  </si>
+  <si>
+    <t>weev_bodyFP_ss.nex</t>
+  </si>
+  <si>
+    <t>weev_neotransFP_ss.nex</t>
   </si>
 </sst>
 </file>
@@ -33316,10 +33331,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33625,53 +33640,33 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="16" customFormat="1">
-      <c r="B9" s="16" t="s">
-        <v>350</v>
-      </c>
-      <c r="C9" s="17">
-        <v>-2241.16</v>
-      </c>
-      <c r="D9" s="17">
-        <v>-2245.3000000000002</v>
-      </c>
-      <c r="E9" s="17">
-        <v>8.34</v>
-      </c>
-      <c r="F9" s="17">
-        <v>-1</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>351</v>
-      </c>
-      <c r="H9" s="55" t="s">
-        <v>958</v>
-      </c>
-      <c r="I9" s="59">
-        <v>221.18</v>
-      </c>
-      <c r="J9" s="19">
-        <v>0.215</v>
-      </c>
-      <c r="K9" s="19">
-        <v>0.79900000000000004</v>
-      </c>
-      <c r="L9" s="71">
-        <v>0.17499999999999999</v>
-      </c>
+    <row r="9" spans="1:13" s="26" customFormat="1">
+      <c r="B9" s="26" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="74"/>
     </row>
     <row r="10" spans="1:13" s="16" customFormat="1">
       <c r="B10" s="16" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C10" s="17">
-        <v>-2471.73</v>
+        <v>-2241.16</v>
       </c>
       <c r="D10" s="17">
-        <v>-2554.5</v>
+        <v>-2245.3000000000002</v>
       </c>
       <c r="E10" s="17">
-        <v>147.72999999999999</v>
+        <v>8.34</v>
       </c>
       <c r="F10" s="17">
         <v>-1</v>
@@ -33683,100 +33678,100 @@
         <v>958</v>
       </c>
       <c r="I10" s="59">
-        <v>120.89</v>
+        <v>221.18</v>
       </c>
       <c r="J10" s="19">
-        <v>0.22500000000000001</v>
+        <v>0.215</v>
       </c>
       <c r="K10" s="19">
-        <v>0.79300000000000004</v>
+        <v>0.79900000000000004</v>
       </c>
       <c r="L10" s="71">
-        <v>0.22750000000000001</v>
+        <v>0.17499999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="16" customFormat="1">
-      <c r="B11" s="32" t="s">
-        <v>940</v>
+      <c r="B11" s="16" t="s">
+        <v>352</v>
       </c>
       <c r="C11" s="17">
-        <v>-2622.36</v>
+        <v>-2471.73</v>
       </c>
       <c r="D11" s="17">
-        <v>-2635.76</v>
+        <v>-2554.5</v>
       </c>
       <c r="E11" s="17">
-        <v>54.19</v>
+        <v>147.72999999999999</v>
       </c>
       <c r="F11" s="17">
         <v>-1</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="18" t="s">
         <v>351</v>
       </c>
       <c r="H11" s="55" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="I11" s="59">
-        <v>52.55</v>
+        <v>120.89</v>
       </c>
       <c r="J11" s="19">
         <v>0.22500000000000001</v>
       </c>
       <c r="K11" s="19">
-        <v>0.79700000000000004</v>
+        <v>0.79300000000000004</v>
       </c>
       <c r="L11" s="71">
-        <v>0.18</v>
+        <v>0.22750000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="16" customFormat="1">
       <c r="B12" s="32" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C12" s="17">
         <v>-2622.36</v>
       </c>
       <c r="D12" s="17">
-        <v>-2649.35</v>
+        <v>-2635.76</v>
       </c>
       <c r="E12" s="17">
-        <v>55.91</v>
+        <v>54.19</v>
       </c>
       <c r="F12" s="17">
         <v>-1</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="31" t="s">
         <v>351</v>
       </c>
       <c r="H12" s="55" t="s">
-        <v>961</v>
-      </c>
-      <c r="I12" s="17">
-        <v>52.6</v>
-      </c>
-      <c r="J12" s="62">
-        <v>0.22600000000000001</v>
+        <v>957</v>
+      </c>
+      <c r="I12" s="59">
+        <v>52.55</v>
+      </c>
+      <c r="J12" s="19">
+        <v>0.22500000000000001</v>
       </c>
       <c r="K12" s="19">
         <v>0.79700000000000004</v>
       </c>
       <c r="L12" s="71">
-        <v>8.2500000000000004E-2</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="16" customFormat="1">
       <c r="B13" s="32" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="C13" s="17">
-        <v>-2525.58</v>
+        <v>-2622.36</v>
       </c>
       <c r="D13" s="17">
-        <v>-2611.0100000000002</v>
+        <v>-2649.35</v>
       </c>
       <c r="E13" s="17">
-        <v>57.44</v>
+        <v>55.91</v>
       </c>
       <c r="F13" s="17">
         <v>-1</v>
@@ -33785,33 +33780,33 @@
         <v>351</v>
       </c>
       <c r="H13" s="55" t="s">
-        <v>957</v>
-      </c>
-      <c r="I13" s="59">
-        <v>87.99</v>
-      </c>
-      <c r="J13" s="19">
-        <v>0.218</v>
+        <v>961</v>
+      </c>
+      <c r="I13" s="17">
+        <v>52.6</v>
+      </c>
+      <c r="J13" s="62">
+        <v>0.22600000000000001</v>
       </c>
       <c r="K13" s="19">
         <v>0.79700000000000004</v>
       </c>
       <c r="L13" s="71">
-        <v>0.39500000000000002</v>
+        <v>8.2500000000000004E-2</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="16" customFormat="1">
       <c r="B14" s="32" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="C14" s="17">
-        <v>-2621.79</v>
+        <v>-2525.58</v>
       </c>
       <c r="D14" s="17">
-        <v>-2635.48</v>
+        <v>-2611.0100000000002</v>
       </c>
       <c r="E14" s="17">
-        <v>56</v>
+        <v>57.44</v>
       </c>
       <c r="F14" s="17">
         <v>-1</v>
@@ -33823,30 +33818,30 @@
         <v>957</v>
       </c>
       <c r="I14" s="59">
-        <v>52.68</v>
+        <v>87.99</v>
       </c>
       <c r="J14" s="19">
-        <v>0.224</v>
+        <v>0.218</v>
       </c>
       <c r="K14" s="19">
         <v>0.79700000000000004</v>
       </c>
       <c r="L14" s="71">
-        <v>8.7499999999999994E-2</v>
+        <v>0.39500000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="16" customFormat="1">
       <c r="B15" s="32" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C15" s="17">
-        <v>-2623.67</v>
+        <v>-2621.79</v>
       </c>
       <c r="D15" s="17">
-        <v>-2663.12</v>
+        <v>-2635.48</v>
       </c>
       <c r="E15" s="17">
-        <v>54.96</v>
+        <v>56</v>
       </c>
       <c r="F15" s="17">
         <v>-1</v>
@@ -33855,103 +33850,83 @@
         <v>351</v>
       </c>
       <c r="H15" s="55" t="s">
-        <v>963</v>
+        <v>957</v>
       </c>
       <c r="I15" s="59">
-        <v>52.17</v>
+        <v>52.68</v>
       </c>
       <c r="J15" s="19">
-        <v>0.22600000000000001</v>
+        <v>0.224</v>
       </c>
       <c r="K15" s="19">
         <v>0.79700000000000004</v>
       </c>
       <c r="L15" s="71">
+        <v>8.7499999999999994E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="16" customFormat="1">
+      <c r="B16" s="32" t="s">
+        <v>944</v>
+      </c>
+      <c r="C16" s="17">
+        <v>-2623.67</v>
+      </c>
+      <c r="D16" s="17">
+        <v>-2663.12</v>
+      </c>
+      <c r="E16" s="17">
+        <v>54.96</v>
+      </c>
+      <c r="F16" s="17">
+        <v>-1</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="H16" s="55" t="s">
+        <v>963</v>
+      </c>
+      <c r="I16" s="59">
+        <v>52.17</v>
+      </c>
+      <c r="J16" s="19">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="K16" s="19">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="L16" s="71">
         <v>0.39500000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="21" customFormat="1">
-      <c r="B16" s="21" t="s">
-        <v>934</v>
-      </c>
-      <c r="C16" s="22">
-        <v>-2347.1999999999998</v>
-      </c>
-      <c r="D16" s="22">
-        <v>-2443.09</v>
-      </c>
-      <c r="E16" s="22">
-        <v>192.63</v>
-      </c>
-      <c r="F16" s="22">
-        <v>-1</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>351</v>
-      </c>
-      <c r="H16" s="56" t="s">
-        <v>958</v>
-      </c>
-      <c r="I16" s="60">
-        <v>184.14</v>
-      </c>
-      <c r="J16" s="24">
-        <v>0.216</v>
-      </c>
-      <c r="K16" s="24">
-        <v>0.79300000000000004</v>
-      </c>
-      <c r="L16" s="72">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="21" customFormat="1">
-      <c r="B17" s="21" t="s">
-        <v>971</v>
-      </c>
-      <c r="C17" s="22">
-        <v>-2538.12</v>
-      </c>
-      <c r="D17" s="22">
-        <v>-2622.3724999999999</v>
-      </c>
-      <c r="E17" s="22">
-        <v>170.89</v>
-      </c>
-      <c r="F17" s="22">
-        <v>-1</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>351</v>
-      </c>
-      <c r="H17" s="56" t="s">
-        <v>961</v>
-      </c>
-      <c r="I17" s="60">
-        <v>111.18</v>
-      </c>
-      <c r="J17" s="24">
-        <v>0.21199999999999999</v>
-      </c>
-      <c r="K17" s="24">
-        <v>0.78700000000000003</v>
-      </c>
-      <c r="L17" s="72">
-        <v>0.2</v>
-      </c>
+    <row r="17" spans="1:13" s="16" customFormat="1">
+      <c r="B17" s="32" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="71"/>
     </row>
     <row r="18" spans="1:13" s="21" customFormat="1">
       <c r="B18" s="21" t="s">
-        <v>972</v>
+        <v>934</v>
       </c>
       <c r="C18" s="22">
-        <v>-2537.1999999999998</v>
+        <v>-2347.1999999999998</v>
       </c>
       <c r="D18" s="22">
-        <v>-2537.4575</v>
+        <v>-2443.09</v>
       </c>
       <c r="E18" s="22">
-        <v>2.0499999999999998</v>
+        <v>192.63</v>
       </c>
       <c r="F18" s="22">
         <v>-1</v>
@@ -33963,30 +33938,30 @@
         <v>958</v>
       </c>
       <c r="I18" s="60">
-        <v>111.116</v>
+        <v>184.14</v>
       </c>
       <c r="J18" s="24">
-        <v>0.21299999999999999</v>
+        <v>0.216</v>
       </c>
       <c r="K18" s="24">
-        <v>0.78900000000000003</v>
+        <v>0.79300000000000004</v>
       </c>
       <c r="L18" s="72">
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="19" spans="1:13" s="21" customFormat="1">
       <c r="B19" s="21" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="C19" s="22">
-        <v>-2538.4</v>
+        <v>-2538.12</v>
       </c>
       <c r="D19" s="22">
-        <v>-2622.1750000000002</v>
+        <v>-2622.3724999999999</v>
       </c>
       <c r="E19" s="22">
-        <v>169.24</v>
+        <v>170.89</v>
       </c>
       <c r="F19" s="22">
         <v>-1</v>
@@ -33998,30 +33973,30 @@
         <v>961</v>
       </c>
       <c r="I19" s="60">
-        <v>111.06480000000001</v>
+        <v>111.18</v>
       </c>
       <c r="J19" s="24">
-        <v>0.214</v>
+        <v>0.21199999999999999</v>
       </c>
       <c r="K19" s="24">
-        <v>0.78900000000000003</v>
+        <v>0.78700000000000003</v>
       </c>
       <c r="L19" s="72">
-        <v>0.42749999999999999</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="21" customFormat="1">
       <c r="B20" s="21" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="C20" s="22">
-        <v>-2539.4</v>
+        <v>-2537.1999999999998</v>
       </c>
       <c r="D20" s="22">
-        <v>-2664.9470000000001</v>
+        <v>-2537.4575</v>
       </c>
       <c r="E20" s="22">
-        <v>169.47</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="F20" s="22">
         <v>-1</v>
@@ -34030,13 +34005,13 @@
         <v>351</v>
       </c>
       <c r="H20" s="56" t="s">
-        <v>963</v>
+        <v>958</v>
       </c>
       <c r="I20" s="60">
-        <v>110.75190000000001</v>
+        <v>111.116</v>
       </c>
       <c r="J20" s="24">
-        <v>0.215</v>
+        <v>0.21299999999999999</v>
       </c>
       <c r="K20" s="24">
         <v>0.78900000000000003</v>
@@ -34047,16 +34022,16 @@
     </row>
     <row r="21" spans="1:13" s="21" customFormat="1">
       <c r="B21" s="21" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="C21" s="22">
-        <v>-2348.15</v>
+        <v>-2538.4</v>
       </c>
       <c r="D21" s="22">
-        <v>-2587.0825</v>
+        <v>-2622.1750000000002</v>
       </c>
       <c r="E21" s="22">
-        <v>360.48</v>
+        <v>169.24</v>
       </c>
       <c r="F21" s="22">
         <v>-1</v>
@@ -34068,214 +34043,191 @@
         <v>961</v>
       </c>
       <c r="I21" s="60">
+        <v>111.06480000000001</v>
+      </c>
+      <c r="J21" s="24">
+        <v>0.214</v>
+      </c>
+      <c r="K21" s="24">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="L21" s="72">
+        <v>0.42749999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="21" customFormat="1">
+      <c r="B22" s="21" t="s">
+        <v>974</v>
+      </c>
+      <c r="C22" s="22">
+        <v>-2539.4</v>
+      </c>
+      <c r="D22" s="22">
+        <v>-2664.9470000000001</v>
+      </c>
+      <c r="E22" s="22">
+        <v>169.47</v>
+      </c>
+      <c r="F22" s="22">
+        <v>-1</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="H22" s="56" t="s">
+        <v>963</v>
+      </c>
+      <c r="I22" s="60">
+        <v>110.75190000000001</v>
+      </c>
+      <c r="J22" s="24">
+        <v>0.215</v>
+      </c>
+      <c r="K22" s="24">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="L22" s="72">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="21" customFormat="1">
+      <c r="B23" s="21" t="s">
+        <v>975</v>
+      </c>
+      <c r="C23" s="22">
+        <v>-2348.15</v>
+      </c>
+      <c r="D23" s="22">
+        <v>-2587.0825</v>
+      </c>
+      <c r="E23" s="22">
+        <v>360.48</v>
+      </c>
+      <c r="F23" s="22">
+        <v>-1</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="H23" s="56" t="s">
+        <v>961</v>
+      </c>
+      <c r="I23" s="60">
         <v>183.7098</v>
       </c>
-      <c r="J21" s="24">
+      <c r="J23" s="24">
         <v>0.21</v>
       </c>
-      <c r="K21" s="24">
+      <c r="K23" s="24">
         <v>0.79</v>
       </c>
-      <c r="L21" s="72">
+      <c r="L23" s="72">
         <v>0.42</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
-      <c r="G22"/>
-    </row>
-    <row r="23" spans="1:13" s="11" customFormat="1">
-      <c r="A23" s="11" t="s">
+    <row r="24" spans="1:13" s="21" customFormat="1">
+      <c r="B24" s="21" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="72"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="1:13" s="11" customFormat="1">
+      <c r="A26" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B26" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C26" s="12">
         <v>-1600.82</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D26" s="12">
         <v>-1601.5</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E26" s="12">
         <v>3.75</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F26" s="12">
         <v>-1</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G26" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H26" s="15" t="s">
         <v>965</v>
       </c>
-      <c r="I23" s="12" t="s">
+      <c r="I26" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="J23" s="14">
+      <c r="J26" s="14">
         <v>0.26</v>
       </c>
-      <c r="K23" s="14">
+      <c r="K26" s="14">
         <v>0.84199999999999997</v>
       </c>
-      <c r="L23" s="70">
+      <c r="L26" s="70">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="11" customFormat="1">
-      <c r="B24" s="11" t="s">
+    <row r="27" spans="1:13" s="11" customFormat="1">
+      <c r="B27" s="11" t="s">
         <v>356</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C27" s="12">
         <v>-1600.05</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D27" s="12">
         <v>-1600.79</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E27" s="12">
         <v>3.29</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F27" s="12">
         <v>-1</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G27" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="H24" s="15" t="s">
+      <c r="H27" s="15" t="s">
         <v>965</v>
       </c>
-      <c r="I24" s="12" t="s">
+      <c r="I27" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="J24" s="14">
+      <c r="J27" s="14">
         <v>0.26800000000000002</v>
       </c>
-      <c r="K24" s="14">
+      <c r="K27" s="14">
         <v>0.84299999999999997</v>
       </c>
-      <c r="L24" s="70">
+      <c r="L27" s="70">
         <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" s="26" customFormat="1">
-      <c r="B25" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="27">
-        <v>-1619.98</v>
-      </c>
-      <c r="D25" s="27">
-        <v>-1622.13</v>
-      </c>
-      <c r="E25" s="27">
-        <v>5.98</v>
-      </c>
-      <c r="F25" s="27">
-        <v>-1</v>
-      </c>
-      <c r="G25" s="28" t="s">
-        <v>349</v>
-      </c>
-      <c r="H25" s="30" t="s">
-        <v>965</v>
-      </c>
-      <c r="I25" s="27" t="s">
-        <v>336</v>
-      </c>
-      <c r="J25" s="29">
-        <v>0.26100000000000001</v>
-      </c>
-      <c r="K25" s="29">
-        <v>0.84199999999999997</v>
-      </c>
-      <c r="L25" s="74">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" s="26" customFormat="1">
-      <c r="B26" s="26" t="s">
-        <v>337</v>
-      </c>
-      <c r="C26" s="27">
-        <v>-1614.56</v>
-      </c>
-      <c r="D26" s="27">
-        <v>-1615.48</v>
-      </c>
-      <c r="E26" s="27">
-        <v>4.49</v>
-      </c>
-      <c r="F26" s="27">
-        <v>-1</v>
-      </c>
-      <c r="G26" s="28" t="s">
-        <v>349</v>
-      </c>
-      <c r="H26" s="30" t="s">
-        <v>965</v>
-      </c>
-      <c r="I26" s="27" t="s">
-        <v>336</v>
-      </c>
-      <c r="J26" s="29">
-        <v>0.26</v>
-      </c>
-      <c r="K26" s="29">
-        <v>0.84099999999999997</v>
-      </c>
-      <c r="L26" s="74">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" s="26" customFormat="1">
-      <c r="B27" s="26" t="s">
-        <v>345</v>
-      </c>
-      <c r="C27" s="27">
-        <v>-1615.29</v>
-      </c>
-      <c r="D27" s="27">
-        <v>-1615.62</v>
-      </c>
-      <c r="E27" s="27">
-        <v>1.87</v>
-      </c>
-      <c r="F27" s="27">
-        <v>-1</v>
-      </c>
-      <c r="G27" s="28" t="s">
-        <v>349</v>
-      </c>
-      <c r="H27" s="30" t="s">
-        <v>965</v>
-      </c>
-      <c r="I27" s="27" t="s">
-        <v>336</v>
-      </c>
-      <c r="J27" s="29">
-        <v>0.26100000000000001</v>
-      </c>
-      <c r="K27" s="29">
-        <v>0.84099999999999997</v>
-      </c>
-      <c r="L27" s="74">
-        <v>4.7500000000000001E-2</v>
-      </c>
-      <c r="M27" s="26" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="26" customFormat="1">
       <c r="B28" s="26" t="s">
-        <v>347</v>
+        <v>25</v>
       </c>
       <c r="C28" s="27">
-        <v>-1613.18</v>
+        <v>-1619.98</v>
       </c>
       <c r="D28" s="27">
-        <v>-1613.94</v>
+        <v>-1622.13</v>
       </c>
       <c r="E28" s="27">
-        <v>2.09</v>
+        <v>5.98</v>
       </c>
       <c r="F28" s="27">
         <v>-1</v>
@@ -34290,7 +34242,7 @@
         <v>336</v>
       </c>
       <c r="J28" s="29">
-        <v>0.26800000000000002</v>
+        <v>0.26100000000000001</v>
       </c>
       <c r="K28" s="29">
         <v>0.84199999999999997</v>
@@ -34298,162 +34250,145 @@
       <c r="L28" s="74">
         <v>0.04</v>
       </c>
-      <c r="M28" s="26" t="s">
+    </row>
+    <row r="29" spans="1:13" s="26" customFormat="1">
+      <c r="B29" s="26" t="s">
+        <v>337</v>
+      </c>
+      <c r="C29" s="27">
+        <v>-1614.56</v>
+      </c>
+      <c r="D29" s="27">
+        <v>-1615.48</v>
+      </c>
+      <c r="E29" s="27">
+        <v>4.49</v>
+      </c>
+      <c r="F29" s="27">
+        <v>-1</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="H29" s="30" t="s">
+        <v>965</v>
+      </c>
+      <c r="I29" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="J29" s="29">
+        <v>0.26</v>
+      </c>
+      <c r="K29" s="29">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="L29" s="74">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="26" customFormat="1">
+      <c r="B30" s="26" t="s">
+        <v>345</v>
+      </c>
+      <c r="C30" s="27">
+        <v>-1615.29</v>
+      </c>
+      <c r="D30" s="27">
+        <v>-1615.62</v>
+      </c>
+      <c r="E30" s="27">
+        <v>1.87</v>
+      </c>
+      <c r="F30" s="27">
+        <v>-1</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="H30" s="30" t="s">
+        <v>965</v>
+      </c>
+      <c r="I30" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="J30" s="29">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="K30" s="29">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="L30" s="74">
+        <v>4.7500000000000001E-2</v>
+      </c>
+      <c r="M30" s="26" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="26" customFormat="1">
+      <c r="B31" s="26" t="s">
+        <v>347</v>
+      </c>
+      <c r="C31" s="27">
+        <v>-1613.18</v>
+      </c>
+      <c r="D31" s="27">
+        <v>-1613.94</v>
+      </c>
+      <c r="E31" s="27">
+        <v>2.09</v>
+      </c>
+      <c r="F31" s="27">
+        <v>-1</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="H31" s="30" t="s">
+        <v>965</v>
+      </c>
+      <c r="I31" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="J31" s="29">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="K31" s="29">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="L31" s="74">
+        <v>0.04</v>
+      </c>
+      <c r="M31" s="26" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="16" customFormat="1">
-      <c r="B29" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="17">
-        <v>-1561.11</v>
-      </c>
-      <c r="D29" s="17">
-        <v>-1601.2650000000001</v>
-      </c>
-      <c r="E29" s="17">
-        <v>57.75</v>
-      </c>
-      <c r="F29" s="17">
-        <v>-1</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>351</v>
-      </c>
-      <c r="H29" s="20" t="s">
-        <v>963</v>
-      </c>
-      <c r="I29" s="17">
-        <v>26.31</v>
-      </c>
-      <c r="J29" s="19">
-        <v>0.26200000000000001</v>
-      </c>
-      <c r="K29" s="19">
-        <v>0.84199999999999997</v>
-      </c>
-      <c r="L29" s="71">
-        <v>4.7500000000000001E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" s="16" customFormat="1">
-      <c r="B30" s="16" t="s">
-        <v>342</v>
-      </c>
-      <c r="C30" s="17">
-        <v>-1581.38</v>
-      </c>
-      <c r="D30" s="17">
-        <v>-1604.5450000000001</v>
-      </c>
-      <c r="E30" s="17">
-        <v>33.49</v>
-      </c>
-      <c r="F30" s="17">
-        <v>-1</v>
-      </c>
-      <c r="G30" s="18" t="s">
-        <v>351</v>
-      </c>
-      <c r="H30" s="20" t="s">
-        <v>963</v>
-      </c>
-      <c r="I30" s="17">
-        <v>25.3</v>
-      </c>
-      <c r="J30" s="19">
-        <v>0.26800000000000002</v>
-      </c>
-      <c r="K30" s="19">
-        <v>0.84199999999999997</v>
-      </c>
-      <c r="L30" s="71">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" s="16" customFormat="1">
-      <c r="B31" s="16" t="s">
-        <v>344</v>
-      </c>
-      <c r="C31" s="17">
-        <v>-1582.34</v>
-      </c>
-      <c r="D31" s="17">
-        <v>-1598.5274999999999</v>
-      </c>
-      <c r="E31" s="17">
-        <v>33.89</v>
-      </c>
-      <c r="F31" s="17">
-        <v>-1</v>
-      </c>
-      <c r="G31" s="18" t="s">
-        <v>351</v>
-      </c>
-      <c r="H31" s="20" t="s">
-        <v>961</v>
-      </c>
-      <c r="I31" s="17">
-        <v>25.443999999999999</v>
-      </c>
-      <c r="J31" s="19">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="K31" s="19">
-        <v>0.84199999999999997</v>
-      </c>
-      <c r="L31" s="71">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" s="16" customFormat="1">
-      <c r="B32" s="16" t="s">
-        <v>946</v>
-      </c>
-      <c r="C32" s="17">
-        <v>-1574.07</v>
-      </c>
-      <c r="D32" s="17">
-        <v>-1588.63</v>
-      </c>
-      <c r="E32" s="17">
-        <v>34.729999999999997</v>
-      </c>
-      <c r="F32" s="17">
-        <v>-1</v>
-      </c>
-      <c r="G32" s="18" t="s">
-        <v>351</v>
-      </c>
-      <c r="H32" s="20" t="s">
-        <v>961</v>
-      </c>
-      <c r="I32" s="17">
-        <v>25.755700000000001</v>
-      </c>
-      <c r="J32" s="19">
-        <v>0.25800000000000001</v>
-      </c>
-      <c r="K32" s="19">
-        <v>0.82899999999999996</v>
-      </c>
-      <c r="L32" s="71">
-        <v>3.2500000000000001E-2</v>
-      </c>
+    <row r="32" spans="1:13" s="26" customFormat="1">
+      <c r="B32" s="26" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="74"/>
     </row>
     <row r="33" spans="2:12" s="16" customFormat="1">
       <c r="B33" s="16" t="s">
-        <v>947</v>
+        <v>30</v>
       </c>
       <c r="C33" s="17">
-        <v>-1576.7</v>
+        <v>-1561.11</v>
       </c>
       <c r="D33" s="17">
-        <v>-1592.81</v>
+        <v>-1601.2650000000001</v>
       </c>
       <c r="E33" s="17">
-        <v>33.659999999999997</v>
+        <v>57.75</v>
       </c>
       <c r="F33" s="17">
         <v>-1</v>
@@ -34462,33 +34397,33 @@
         <v>351</v>
       </c>
       <c r="H33" s="20" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="I33" s="17">
-        <v>25.21</v>
+        <v>26.31</v>
       </c>
       <c r="J33" s="19">
-        <v>0.26</v>
+        <v>0.26200000000000001</v>
       </c>
       <c r="K33" s="19">
-        <v>0.82899999999999996</v>
+        <v>0.84199999999999997</v>
       </c>
       <c r="L33" s="71">
-        <v>2.5000000000000001E-3</v>
+        <v>4.7500000000000001E-2</v>
       </c>
     </row>
     <row r="34" spans="2:12" s="16" customFormat="1">
       <c r="B34" s="16" t="s">
-        <v>948</v>
+        <v>342</v>
       </c>
       <c r="C34" s="17">
-        <v>-1573.44</v>
+        <v>-1581.38</v>
       </c>
       <c r="D34" s="17">
-        <v>-1597.19</v>
+        <v>-1604.5450000000001</v>
       </c>
       <c r="E34" s="17">
-        <v>34.799999999999997</v>
+        <v>33.49</v>
       </c>
       <c r="F34" s="17">
         <v>-1</v>
@@ -34500,65 +34435,65 @@
         <v>963</v>
       </c>
       <c r="I34" s="17">
-        <v>25.925699999999999</v>
+        <v>25.3</v>
       </c>
       <c r="J34" s="19">
-        <v>0.26</v>
+        <v>0.26800000000000002</v>
       </c>
       <c r="K34" s="19">
-        <v>0.82899999999999996</v>
+        <v>0.84199999999999997</v>
       </c>
       <c r="L34" s="71">
-        <v>0.19500000000000001</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="35" spans="2:12" s="16" customFormat="1">
       <c r="B35" s="16" t="s">
-        <v>949</v>
+        <v>344</v>
       </c>
       <c r="C35" s="17">
-        <v>-1602.5</v>
+        <v>-1582.34</v>
       </c>
       <c r="D35" s="17">
-        <v>-1606.1849999999999</v>
+        <v>-1598.5274999999999</v>
       </c>
       <c r="E35" s="17">
-        <v>7.34</v>
+        <v>33.89</v>
       </c>
       <c r="F35" s="17">
         <v>-1</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>965</v>
-      </c>
-      <c r="I35" s="17" t="s">
-        <v>336</v>
+        <v>961</v>
+      </c>
+      <c r="I35" s="17">
+        <v>25.443999999999999</v>
       </c>
       <c r="J35" s="19">
-        <v>0.26100000000000001</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="K35" s="19">
-        <v>0.83</v>
+        <v>0.84199999999999997</v>
       </c>
       <c r="L35" s="71">
-        <v>5.0000000000000001E-3</v>
+        <v>4.2500000000000003E-2</v>
       </c>
     </row>
     <row r="36" spans="2:12" s="16" customFormat="1">
       <c r="B36" s="16" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
       <c r="C36" s="17">
-        <v>-1573.15</v>
+        <v>-1574.07</v>
       </c>
       <c r="D36" s="17">
-        <v>-1596.8025</v>
+        <v>-1588.63</v>
       </c>
       <c r="E36" s="17">
-        <v>35.36</v>
+        <v>34.729999999999997</v>
       </c>
       <c r="F36" s="17">
         <v>-1</v>
@@ -34567,306 +34502,476 @@
         <v>351</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="I36" s="17">
-        <v>25.513000000000002</v>
+        <v>25.755700000000001</v>
       </c>
       <c r="J36" s="19">
         <v>0.25800000000000001</v>
       </c>
       <c r="K36" s="19">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="L36" s="71">
+        <v>3.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" s="16" customFormat="1">
+      <c r="B37" s="16" t="s">
+        <v>947</v>
+      </c>
+      <c r="C37" s="17">
+        <v>-1576.7</v>
+      </c>
+      <c r="D37" s="17">
+        <v>-1592.81</v>
+      </c>
+      <c r="E37" s="17">
+        <v>33.659999999999997</v>
+      </c>
+      <c r="F37" s="17">
+        <v>-1</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="H37" s="20" t="s">
+        <v>961</v>
+      </c>
+      <c r="I37" s="17">
+        <v>25.21</v>
+      </c>
+      <c r="J37" s="19">
+        <v>0.26</v>
+      </c>
+      <c r="K37" s="19">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="L37" s="71">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" s="16" customFormat="1">
+      <c r="B38" s="16" t="s">
+        <v>948</v>
+      </c>
+      <c r="C38" s="17">
+        <v>-1573.44</v>
+      </c>
+      <c r="D38" s="17">
+        <v>-1597.19</v>
+      </c>
+      <c r="E38" s="17">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="F38" s="17">
+        <v>-1</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="H38" s="20" t="s">
+        <v>963</v>
+      </c>
+      <c r="I38" s="17">
+        <v>25.925699999999999</v>
+      </c>
+      <c r="J38" s="19">
+        <v>0.26</v>
+      </c>
+      <c r="K38" s="19">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="L38" s="71">
+        <v>0.19500000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" s="16" customFormat="1">
+      <c r="B39" s="16" t="s">
+        <v>949</v>
+      </c>
+      <c r="C39" s="17">
+        <v>-1602.5</v>
+      </c>
+      <c r="D39" s="17">
+        <v>-1606.1849999999999</v>
+      </c>
+      <c r="E39" s="17">
+        <v>7.34</v>
+      </c>
+      <c r="F39" s="17">
+        <v>-1</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>965</v>
+      </c>
+      <c r="I39" s="17" t="s">
+        <v>336</v>
+      </c>
+      <c r="J39" s="19">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="K39" s="19">
         <v>0.83</v>
       </c>
-      <c r="L36" s="71">
+      <c r="L39" s="71">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" s="16" customFormat="1">
+      <c r="B40" s="16" t="s">
+        <v>950</v>
+      </c>
+      <c r="C40" s="17">
+        <v>-1573.15</v>
+      </c>
+      <c r="D40" s="17">
+        <v>-1596.8025</v>
+      </c>
+      <c r="E40" s="17">
+        <v>35.36</v>
+      </c>
+      <c r="F40" s="17">
+        <v>-1</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>963</v>
+      </c>
+      <c r="I40" s="17">
+        <v>25.513000000000002</v>
+      </c>
+      <c r="J40" s="19">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="K40" s="19">
+        <v>0.83</v>
+      </c>
+      <c r="L40" s="71">
         <v>0.19</v>
       </c>
     </row>
-    <row r="37" spans="2:12" s="21" customFormat="1">
-      <c r="B37" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="22">
-        <v>-1578.28</v>
-      </c>
-      <c r="D37" s="22">
-        <v>-1578.22</v>
-      </c>
-      <c r="E37" s="22">
-        <v>4.05</v>
-      </c>
-      <c r="F37" s="22">
-        <v>-1</v>
-      </c>
-      <c r="G37" s="23" t="s">
-        <v>351</v>
-      </c>
-      <c r="H37" s="25" t="s">
-        <v>958</v>
-      </c>
-      <c r="I37" s="22">
-        <v>30.8</v>
-      </c>
-      <c r="J37" s="24">
-        <v>0.26200000000000001</v>
-      </c>
-      <c r="K37" s="24">
-        <v>0.84199999999999997</v>
-      </c>
-      <c r="L37" s="72">
-        <v>4.4999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" s="21" customFormat="1">
-      <c r="B38" s="21" t="s">
-        <v>341</v>
-      </c>
-      <c r="C38" s="22">
-        <v>-1575.69</v>
-      </c>
-      <c r="D38" s="22">
-        <v>-1595.39</v>
-      </c>
-      <c r="E38" s="22">
-        <v>41.97</v>
-      </c>
-      <c r="F38" s="22">
-        <v>-1</v>
-      </c>
-      <c r="G38" s="23" t="s">
-        <v>351</v>
-      </c>
-      <c r="H38" s="25" t="s">
-        <v>961</v>
-      </c>
-      <c r="I38" s="22">
-        <v>30.52</v>
-      </c>
-      <c r="J38" s="24">
-        <v>0.25700000000000001</v>
-      </c>
-      <c r="K38" s="24">
-        <v>0.84099999999999997</v>
-      </c>
-      <c r="L38" s="72">
-        <v>4.4999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12" s="21" customFormat="1">
-      <c r="B39" s="21" t="s">
-        <v>343</v>
-      </c>
-      <c r="C39" s="22">
-        <v>-1576.36</v>
-      </c>
-      <c r="D39" s="22">
-        <v>-1577.88</v>
-      </c>
-      <c r="E39" s="22">
-        <v>4.57</v>
-      </c>
-      <c r="F39" s="22">
-        <v>-1</v>
-      </c>
-      <c r="G39" s="23" t="s">
-        <v>351</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>958</v>
-      </c>
-      <c r="I39" s="22">
-        <v>30.9</v>
-      </c>
-      <c r="J39" s="24">
-        <v>0.26700000000000002</v>
-      </c>
-      <c r="K39" s="24">
-        <v>0.84299999999999997</v>
-      </c>
-      <c r="L39" s="72">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" s="21" customFormat="1">
-      <c r="B40" s="21" t="s">
-        <v>966</v>
-      </c>
-      <c r="C40" s="22">
-        <v>-1573.67</v>
-      </c>
-      <c r="D40" s="22">
-        <v>-1587.4124999999999</v>
-      </c>
-      <c r="E40" s="22">
-        <v>43.79</v>
-      </c>
-      <c r="F40" s="22">
-        <v>-1</v>
-      </c>
-      <c r="G40" s="75" t="s">
-        <v>351</v>
-      </c>
-      <c r="H40" s="56" t="s">
-        <v>957</v>
-      </c>
-      <c r="I40" s="60">
-        <v>31.0885</v>
-      </c>
-      <c r="J40" s="24">
-        <v>0.255</v>
-      </c>
-      <c r="K40" s="24">
-        <v>0.83899999999999997</v>
-      </c>
-      <c r="L40" s="72">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" s="21" customFormat="1">
-      <c r="B41" s="21" t="s">
-        <v>967</v>
-      </c>
-      <c r="C41" s="22">
-        <v>-1582.11</v>
-      </c>
-      <c r="D41" s="22">
-        <v>-1608.7950000000001</v>
-      </c>
-      <c r="E41" s="22">
-        <v>39.42</v>
-      </c>
-      <c r="F41" s="22">
-        <v>-1</v>
-      </c>
-      <c r="G41" s="75" t="s">
-        <v>351</v>
-      </c>
-      <c r="H41" s="56" t="s">
-        <v>963</v>
-      </c>
-      <c r="I41" s="60">
-        <v>30.580200000000001</v>
-      </c>
-      <c r="J41" s="24">
-        <v>0.25900000000000001</v>
-      </c>
-      <c r="K41" s="24">
-        <v>0.83799999999999997</v>
-      </c>
-      <c r="L41" s="72">
-        <v>0.01</v>
-      </c>
+    <row r="41" spans="2:12" s="16" customFormat="1">
+      <c r="B41" s="16" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="71"/>
     </row>
     <row r="42" spans="2:12" s="21" customFormat="1">
       <c r="B42" s="21" t="s">
-        <v>968</v>
+        <v>32</v>
       </c>
       <c r="C42" s="22">
-        <v>-1578.08</v>
+        <v>-1578.28</v>
       </c>
       <c r="D42" s="22">
-        <v>-1589</v>
+        <v>-1578.22</v>
       </c>
       <c r="E42" s="22">
-        <v>41.44</v>
+        <v>4.05</v>
       </c>
       <c r="F42" s="22">
         <v>-1</v>
       </c>
-      <c r="G42" s="75" t="s">
+      <c r="G42" s="23" t="s">
         <v>351</v>
       </c>
-      <c r="H42" s="56" t="s">
-        <v>957</v>
-      </c>
-      <c r="I42" s="60">
-        <v>31.096699999999998</v>
+      <c r="H42" s="25" t="s">
+        <v>958</v>
+      </c>
+      <c r="I42" s="22">
+        <v>30.8</v>
       </c>
       <c r="J42" s="24">
-        <v>0.26100000000000001</v>
+        <v>0.26200000000000001</v>
       </c>
       <c r="K42" s="24">
-        <v>0.83799999999999997</v>
+        <v>0.84199999999999997</v>
       </c>
       <c r="L42" s="72">
-        <v>0.23</v>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="43" spans="2:12" s="21" customFormat="1">
       <c r="B43" s="21" t="s">
-        <v>969</v>
+        <v>341</v>
       </c>
       <c r="C43" s="22">
-        <v>-1577.91</v>
+        <v>-1575.69</v>
       </c>
       <c r="D43" s="22">
-        <v>-1587.7925</v>
+        <v>-1595.39</v>
       </c>
       <c r="E43" s="22">
-        <v>40.4</v>
+        <v>41.97</v>
       </c>
       <c r="F43" s="22">
         <v>-1</v>
       </c>
-      <c r="G43" s="75" t="s">
+      <c r="G43" s="23" t="s">
         <v>351</v>
       </c>
-      <c r="H43" s="56" t="s">
-        <v>957</v>
-      </c>
-      <c r="I43" s="60">
-        <v>30.961500000000001</v>
+      <c r="H43" s="25" t="s">
+        <v>961</v>
+      </c>
+      <c r="I43" s="22">
+        <v>30.52</v>
       </c>
       <c r="J43" s="24">
-        <v>0.255</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="K43" s="24">
-        <v>0.83899999999999997</v>
+        <v>0.84099999999999997</v>
       </c>
       <c r="L43" s="72">
-        <v>0.1</v>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="44" spans="2:12" s="21" customFormat="1">
       <c r="B44" s="21" t="s">
-        <v>970</v>
+        <v>343</v>
       </c>
       <c r="C44" s="22">
-        <v>-1578.14</v>
+        <v>-1576.36</v>
       </c>
       <c r="D44" s="22">
-        <v>-1596.7170000000001</v>
+        <v>-1577.88</v>
       </c>
       <c r="E44" s="22">
-        <v>39.61</v>
+        <v>4.57</v>
       </c>
       <c r="F44" s="22">
         <v>-1</v>
       </c>
-      <c r="G44" s="75" t="s">
+      <c r="G44" s="23" t="s">
         <v>351</v>
       </c>
-      <c r="H44" s="56" t="s">
+      <c r="H44" s="25" t="s">
+        <v>958</v>
+      </c>
+      <c r="I44" s="22">
+        <v>30.9</v>
+      </c>
+      <c r="J44" s="24">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="K44" s="24">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="L44" s="72">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" s="21" customFormat="1">
+      <c r="B45" s="21" t="s">
+        <v>966</v>
+      </c>
+      <c r="C45" s="22">
+        <v>-1573.67</v>
+      </c>
+      <c r="D45" s="22">
+        <v>-1587.4124999999999</v>
+      </c>
+      <c r="E45" s="22">
+        <v>43.79</v>
+      </c>
+      <c r="F45" s="22">
+        <v>-1</v>
+      </c>
+      <c r="G45" s="75" t="s">
+        <v>351</v>
+      </c>
+      <c r="H45" s="56" t="s">
+        <v>957</v>
+      </c>
+      <c r="I45" s="60">
+        <v>31.0885</v>
+      </c>
+      <c r="J45" s="24">
+        <v>0.255</v>
+      </c>
+      <c r="K45" s="24">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="L45" s="72">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" s="21" customFormat="1">
+      <c r="B46" s="21" t="s">
+        <v>967</v>
+      </c>
+      <c r="C46" s="22">
+        <v>-1582.11</v>
+      </c>
+      <c r="D46" s="22">
+        <v>-1608.7950000000001</v>
+      </c>
+      <c r="E46" s="22">
+        <v>39.42</v>
+      </c>
+      <c r="F46" s="22">
+        <v>-1</v>
+      </c>
+      <c r="G46" s="75" t="s">
+        <v>351</v>
+      </c>
+      <c r="H46" s="56" t="s">
+        <v>963</v>
+      </c>
+      <c r="I46" s="60">
+        <v>30.580200000000001</v>
+      </c>
+      <c r="J46" s="24">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="K46" s="24">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="L46" s="72">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" s="21" customFormat="1">
+      <c r="B47" s="21" t="s">
+        <v>968</v>
+      </c>
+      <c r="C47" s="22">
+        <v>-1578.08</v>
+      </c>
+      <c r="D47" s="22">
+        <v>-1589</v>
+      </c>
+      <c r="E47" s="22">
+        <v>41.44</v>
+      </c>
+      <c r="F47" s="22">
+        <v>-1</v>
+      </c>
+      <c r="G47" s="75" t="s">
+        <v>351</v>
+      </c>
+      <c r="H47" s="56" t="s">
+        <v>957</v>
+      </c>
+      <c r="I47" s="60">
+        <v>31.096699999999998</v>
+      </c>
+      <c r="J47" s="24">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="K47" s="24">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="L47" s="72">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" s="21" customFormat="1">
+      <c r="B48" s="21" t="s">
+        <v>969</v>
+      </c>
+      <c r="C48" s="22">
+        <v>-1577.91</v>
+      </c>
+      <c r="D48" s="22">
+        <v>-1587.7925</v>
+      </c>
+      <c r="E48" s="22">
+        <v>40.4</v>
+      </c>
+      <c r="F48" s="22">
+        <v>-1</v>
+      </c>
+      <c r="G48" s="75" t="s">
+        <v>351</v>
+      </c>
+      <c r="H48" s="56" t="s">
+        <v>957</v>
+      </c>
+      <c r="I48" s="60">
+        <v>30.961500000000001</v>
+      </c>
+      <c r="J48" s="24">
+        <v>0.255</v>
+      </c>
+      <c r="K48" s="24">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="L48" s="72">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" s="21" customFormat="1">
+      <c r="B49" s="21" t="s">
+        <v>970</v>
+      </c>
+      <c r="C49" s="22">
+        <v>-1578.14</v>
+      </c>
+      <c r="D49" s="22">
+        <v>-1596.7170000000001</v>
+      </c>
+      <c r="E49" s="22">
+        <v>39.61</v>
+      </c>
+      <c r="F49" s="22">
+        <v>-1</v>
+      </c>
+      <c r="G49" s="75" t="s">
+        <v>351</v>
+      </c>
+      <c r="H49" s="56" t="s">
         <v>961</v>
       </c>
-      <c r="I44" s="60">
+      <c r="I49" s="60">
         <v>30.998000000000001</v>
       </c>
-      <c r="J44" s="24">
+      <c r="J49" s="24">
         <v>0.25900000000000001</v>
       </c>
-      <c r="K44" s="24">
+      <c r="K49" s="24">
         <v>0.83899999999999997</v>
       </c>
-      <c r="L44" s="72">
+      <c r="L49" s="72">
         <v>0.23250000000000001</v>
       </c>
+    </row>
+    <row r="50" spans="2:12" s="21" customFormat="1">
+      <c r="B50" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="75"/>
+      <c r="H50" s="56"/>
+      <c r="I50" s="60"/>
+      <c r="J50" s="24"/>
+      <c r="K50" s="24"/>
+      <c r="L50" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="J1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="G12:G1048576 G1:G10">
+  <conditionalFormatting sqref="G13:G1048576 G1:G11">
     <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"no"</formula>
     </cfRule>
@@ -34879,12 +34984,12 @@
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L21 L23:L39">
+  <conditionalFormatting sqref="L2:L24 L26:L44">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L40:L44">
+  <conditionalFormatting sqref="L45:L50">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0.1</formula>
     </cfRule>
@@ -36490,7 +36595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>

</xml_diff>